<commit_message>
Fixed some issues with unicode and json, and column names and some entries; but needs to fix the issue with returning strings for numeric values
</commit_message>
<xml_diff>
--- a/json-example.xlsx
+++ b/json-example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gdhvinca-my.sharepoint.com/personal/jmnam_gdhl_co_kr/Documents/바탕 화면/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gdhvinca-my.sharepoint.com/personal/jmnam_gdhl_co_kr/Documents/문서/Python Scripts/get_currency/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{827C7A98-AE10-449F-8526-DD2EF9A34A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{827C7A98-AE10-449F-8526-DD2EF9A34A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D165B866-1770-488D-9B39-39673F508A03}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FC48D891-3075-4B0A-A352-45D2FFEEDD1D}"/>
   </bookViews>
@@ -62,18 +62,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Cross Rate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cross%20Rate(US$)</t>
-  </si>
-  <si>
     <t>2024-01-15/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>http://127.0.0.1:5000/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Keys</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KRW-USD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -158,6 +159,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -457,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63678C7-081F-48A0-AB27-5B7F6B4D47D1}">
-  <dimension ref="B5:F9"/>
+  <dimension ref="B5:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -482,12 +487,12 @@
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -496,23 +501,29 @@
         <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" t="str">
-        <f>_xlfn.CONCAT(B6,D6,E6,F6,"-1")</f>
-        <v>http://127.0.0.1:5000/get_sub_data/2024-01-15/Cross%20Rate(US$)-1</v>
+        <f>_xlfn.CONCAT(B6,C6,E6,F6)</f>
+        <v>http://127.0.0.1:5000/get_main_data/2024-01-15/KRW-USD</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" t="str">
         <f>_xlfn.WEBSERVICE(B8)</f>
-        <v xml:space="preserve">"1.09470"
+        <v xml:space="preserve">"1,314.10"
 </v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <f>VALUE(SUBSTITUTE(SUBSTITUTE(B9, CHAR(34), ""), CHAR(10), ""))</f>
+        <v>1314.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added examples; fixed numeric issue but still not fixed in excel. Needs to do manually
</commit_message>
<xml_diff>
--- a/json-example.xlsx
+++ b/json-example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gdhvinca-my.sharepoint.com/personal/jmnam_gdhl_co_kr/Documents/문서/Python Scripts/get_currency/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{827C7A98-AE10-449F-8526-DD2EF9A34A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D165B866-1770-488D-9B39-39673F508A03}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="8_{827C7A98-AE10-449F-8526-DD2EF9A34A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06390157-4761-43EA-83CE-95136BB2D2B6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FC48D891-3075-4B0A-A352-45D2FFEEDD1D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>URL</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,6 +75,24 @@
   </si>
   <si>
     <t>KRW-USD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get_rus_data/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/get_rus_data/2024-01-26/Rate-USD</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/get_rus_data/2024-01-15/Rate-USD</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/get_main_data/2024-01-15/KRW-USD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -133,7 +151,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -141,6 +159,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -159,10 +180,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -462,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63678C7-081F-48A0-AB27-5B7F6B4D47D1}">
-  <dimension ref="B5:F10"/>
+  <dimension ref="B5:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -473,7 +490,7 @@
     <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -484,13 +501,16 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
@@ -500,30 +520,101 @@
       <c r="D6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" t="str">
-        <f>_xlfn.CONCAT(B6,C6,E6,F6)</f>
+        <f>_xlfn.CONCAT(B6,C6,F6,G6)</f>
         <v>http://127.0.0.1:5000/get_main_data/2024-01-15/KRW-USD</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" t="str">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" t="str">
         <f>_xlfn.WEBSERVICE(B8)</f>
-        <v xml:space="preserve">"1,314.10"
+        <v xml:space="preserve">1314.1
 </v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(B9, CHAR(34), ""), CHAR(10), ""))</f>
+      <c r="C10">
+        <f>TYPE(B10)</f>
+        <v>2</v>
+      </c>
+      <c r="D10" t="str">
+        <f>SUBSTITUTE(B10, CHAR(10), "")</f>
         <v>1314.1</v>
+      </c>
+      <c r="E10" t="str">
+        <f>TEXT(D10, "0.00")</f>
+        <v>1314.10</v>
+      </c>
+      <c r="F10">
+        <f>TYPE(E10)</f>
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <f>E10*1</f>
+        <v>1314.1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" t="str">
+        <f>_xlfn.WEBSERVICE(B9)</f>
+        <v xml:space="preserve">88.6562
+</v>
+      </c>
+      <c r="C11">
+        <f>TYPE(B11)</f>
+        <v>2</v>
+      </c>
+      <c r="D11" t="str">
+        <f>SUBSTITUTE(B11, CHAR(10), "")</f>
+        <v>88.6562</v>
+      </c>
+      <c r="E11" t="str">
+        <f>TEXT(D11, "0.0000")</f>
+        <v>88.6562</v>
+      </c>
+      <c r="F11">
+        <f>TYPE(E11)</f>
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <f>E11*1</f>
+        <v>88.656199999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" t="str">
+        <f>TEXT(VALUE(SUBSTITUTE(_xlfn.WEBSERVICE(B13), CHAR(10), "")), "0.00")</f>
+        <v>1314.10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" t="str">
+        <f>TEXT(VALUE(SUBSTITUTE(_xlfn.WEBSERVICE(B15), CHAR(10), "")), "0.0000")</f>
+        <v>88.1324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor change in example
</commit_message>
<xml_diff>
--- a/json-example.xlsx
+++ b/json-example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gdhvinca-my.sharepoint.com/personal/jmnam_gdhl_co_kr/Documents/문서/Python Scripts/get_currency/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{827C7A98-AE10-449F-8526-DD2EF9A34A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06390157-4761-43EA-83CE-95136BB2D2B6}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="8_{827C7A98-AE10-449F-8526-DD2EF9A34A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{936EAD4F-58BE-4F57-A3ED-376DF28BBF6C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FC48D891-3075-4B0A-A352-45D2FFEEDD1D}"/>
   </bookViews>
@@ -479,18 +479,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63678C7-081F-48A0-AB27-5B7F6B4D47D1}">
-  <dimension ref="B5:G16"/>
+  <dimension ref="B5:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -509,8 +510,11 @@
       <c r="G5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I5" s="1">
+        <v>45306</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
@@ -529,19 +533,23 @@
       <c r="G6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I6" t="str">
+        <f>"http://124.55.158.229:4752/get_main_data/" &amp; TEXT(I5, "yyyy-mm-dd") &amp; "/KRW-USD"</f>
+        <v>http://124.55.158.229:4752/get_main_data/2024-01-15/KRW-USD</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" t="str">
         <f>_xlfn.CONCAT(B6,C6,F6,G6)</f>
         <v>http://127.0.0.1:5000/get_main_data/2024-01-15/KRW-USD</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" t="str">
         <f>_xlfn.WEBSERVICE(B8)</f>
         <v xml:space="preserve">1314.1
@@ -568,7 +576,7 @@
         <v>1314.1</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
         <f>_xlfn.WEBSERVICE(B9)</f>
         <v xml:space="preserve">88.6562
@@ -595,23 +603,23 @@
         <v>88.656199999999998</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
         <f>TEXT(VALUE(SUBSTITUTE(_xlfn.WEBSERVICE(B13), CHAR(10), "")), "0.00")</f>
         <v>1314.10</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" t="str">
         <f>TEXT(VALUE(SUBSTITUTE(_xlfn.WEBSERVICE(B15), CHAR(10), "")), "0.0000")</f>
         <v>88.1324</v>

</xml_diff>